<commit_message>
added data to Portfolio sheet
</commit_message>
<xml_diff>
--- a/workbooks/total-data.xlsx
+++ b/workbooks/total-data.xlsx
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15499.79256592374</v>
+        <v>15846.72661073366</v>
       </c>
       <c r="C2" t="n">
         <v>12084.38</v>
@@ -5335,7 +5335,7 @@
         <v>12273.445639</v>
       </c>
       <c r="D2" t="n">
-        <v>7375.391355284367</v>
+        <v>7589.280446966309</v>
       </c>
     </row>
     <row r="3">
@@ -5348,7 +5348,7 @@
         <v>81520.14529455001</v>
       </c>
       <c r="D3" t="n">
-        <v>8124.401210639377</v>
+        <v>8257.446163767348</v>
       </c>
     </row>
     <row r="4">
@@ -21927,7 +21927,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>68151.49733752001</v>
+        <v>70913.2391512</v>
       </c>
     </row>
     <row r="3">
@@ -21937,7 +21937,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3456.71105052</v>
+        <v>3563.43113707</v>
       </c>
     </row>
     <row r="4">
@@ -21947,7 +21947,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>165.4500736</v>
+        <v>172.64010102</v>
       </c>
     </row>
     <row r="5">
@@ -21957,7 +21957,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.60305288</v>
+        <v>0.61834962</v>
       </c>
     </row>
     <row r="6">
@@ -21967,7 +21967,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.003758</v>
+        <v>0.99949093</v>
       </c>
     </row>
     <row r="7">
@@ -21977,7 +21977,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.18495618</v>
+        <v>0.19766351</v>
       </c>
     </row>
     <row r="8">
@@ -21987,7 +21987,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.56832611</v>
+        <v>0.5867380800000001</v>
       </c>
     </row>
     <row r="9">
@@ -21997,7 +21997,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46.03771259</v>
+        <v>46.84048265</v>
       </c>
     </row>
     <row r="10">
@@ -22007,7 +22007,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17.10208167</v>
+        <v>17.40671795</v>
       </c>
     </row>
     <row r="11">
@@ -22017,7 +22017,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.86754421</v>
+        <v>0.88396186</v>
       </c>
     </row>
     <row r="12">
@@ -22027,7 +22027,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8.332391680000001</v>
+        <v>8.5253409</v>
       </c>
     </row>
     <row r="13">
@@ -22037,7 +22037,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10.61573592</v>
+        <v>10.84413363</v>
       </c>
     </row>
     <row r="14">
@@ -22047,7 +22047,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.43978758</v>
+        <v>1.46256668</v>
       </c>
     </row>
     <row r="15">
@@ -22057,27 +22057,27 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.12740758</v>
+        <v>0.13024068</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8.98756513</v>
+        <v>0.10129332</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.10014683</v>
+        <v>9.10782049</v>
       </c>
     </row>
     <row r="18">
@@ -22087,7 +22087,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.31852093</v>
+        <v>0.32215476</v>
       </c>
     </row>
     <row r="19">
@@ -22097,7 +22097,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.99031116</v>
+        <v>3.02552795</v>
       </c>
     </row>
     <row r="20">
@@ -22107,7 +22107,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2.48001298</v>
+        <v>2.64157126</v>
       </c>
     </row>
     <row r="21">
@@ -22117,7 +22117,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.05749399</v>
+        <v>0.06011845</v>
       </c>
     </row>
     <row r="22">
@@ -22127,7 +22127,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.22222036</v>
+        <v>0.23007679</v>
       </c>
     </row>
     <row r="23">
@@ -22137,7 +22137,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>114.85446359</v>
+        <v>116.64835414</v>
       </c>
     </row>
     <row r="24">
@@ -22147,7 +22147,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.07661734000000001</v>
+        <v>0.07617235999999999</v>
       </c>
     </row>
     <row r="25">
@@ -22157,7 +22157,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0574323</v>
+        <v>0.05969575</v>
       </c>
     </row>
     <row r="26">
@@ -22167,7 +22167,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.008822139999999999</v>
+        <v>0.00903178</v>
       </c>
     </row>
     <row r="27">
@@ -22177,7 +22177,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.03542987</v>
+        <v>0.03647589</v>
       </c>
     </row>
     <row r="28">
@@ -22187,7 +22187,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.37379499</v>
+        <v>0.38449204</v>
       </c>
     </row>
     <row r="29">
@@ -22197,7 +22197,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.03278477</v>
+        <v>0.03386861</v>
       </c>
     </row>
     <row r="30">
@@ -22207,7 +22207,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.00109943</v>
+        <v>0.00116182</v>
       </c>
     </row>
     <row r="31">
@@ -22217,37 +22217,37 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.1756553</v>
+        <v>0.17793724</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CLV</t>
+          <t>TRAC</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.10010413</v>
+        <v>4.17479172</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GODS</t>
+          <t>CLV</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.28158107</v>
+        <v>0.10572851</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TRAC</t>
+          <t>GODS</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3.75985225</v>
+        <v>0.29279337</v>
       </c>
     </row>
     <row r="35">
@@ -22257,7 +22257,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.08436183999999999</v>
+        <v>0.08835073</v>
       </c>
     </row>
     <row r="36">
@@ -22267,7 +22267,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>100.43664246</v>
+        <v>105.26056</v>
       </c>
     </row>
     <row r="37">
@@ -22277,7 +22277,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.10127998</v>
+        <v>0.10661435</v>
       </c>
     </row>
     <row r="38">
@@ -22287,7 +22287,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.44468181</v>
+        <v>0.46123181</v>
       </c>
     </row>
     <row r="39">
@@ -22297,7 +22297,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.25747821</v>
+        <v>0.24116024</v>
       </c>
     </row>
     <row r="40">
@@ -22307,7 +22307,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02910634</v>
+        <v>0.03041209</v>
       </c>
     </row>
     <row r="41">
@@ -22317,7 +22317,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.0349178</v>
+        <v>0.03870927</v>
       </c>
     </row>
     <row r="42">
@@ -22327,7 +22327,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.01073422</v>
+        <v>0.01216481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made pdf functions to extract data from 8494 forms
</commit_message>
<xml_diff>
--- a/workbooks/total-data.xlsx
+++ b/workbooks/total-data.xlsx
@@ -21927,7 +21927,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70913.2391512</v>
+        <v>70821.43589851</v>
       </c>
     </row>
     <row r="3">
@@ -21937,7 +21937,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3563.43113707</v>
+        <v>3560.3747093</v>
       </c>
     </row>
     <row r="4">
@@ -21947,7 +21947,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>172.64010102</v>
+        <v>172.47016777</v>
       </c>
     </row>
     <row r="5">
@@ -21957,7 +21957,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.61834962</v>
+        <v>0.6139202499999999</v>
       </c>
     </row>
     <row r="6">
@@ -21967,7 +21967,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.99949093</v>
+        <v>1.00109421</v>
       </c>
     </row>
     <row r="7">
@@ -21977,7 +21977,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.19766351</v>
+        <v>0.19458112</v>
       </c>
     </row>
     <row r="8">
@@ -21987,7 +21987,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5867380800000001</v>
+        <v>0.58759816</v>
       </c>
     </row>
     <row r="9">
@@ -21997,7 +21997,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46.84048265</v>
+        <v>46.46327972</v>
       </c>
     </row>
     <row r="10">
@@ -22007,7 +22007,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17.40671795</v>
+        <v>17.36079088</v>
       </c>
     </row>
     <row r="11">
@@ -22017,7 +22017,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.88396186</v>
+        <v>0.88029062</v>
       </c>
     </row>
     <row r="12">
@@ -22027,7 +22027,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8.5253409</v>
+        <v>8.233411090000001</v>
       </c>
     </row>
     <row r="13">
@@ -22037,7 +22037,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10.84413363</v>
+        <v>10.75846816</v>
       </c>
     </row>
     <row r="14">
@@ -22047,7 +22047,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.46256668</v>
+        <v>1.45154211</v>
       </c>
     </row>
     <row r="15">
@@ -22057,7 +22057,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.13024068</v>
+        <v>0.13015978</v>
       </c>
     </row>
     <row r="16">
@@ -22067,7 +22067,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.10129332</v>
+        <v>0.10069435</v>
       </c>
     </row>
     <row r="17">
@@ -22077,27 +22077,27 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9.10782049</v>
+        <v>9.07820976</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GRT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.32215476</v>
+        <v>2.9919456</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>GRT</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3.02552795</v>
+        <v>0.31789509</v>
       </c>
     </row>
     <row r="20">
@@ -22107,7 +22107,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2.64157126</v>
+        <v>2.59994953</v>
       </c>
     </row>
     <row r="21">
@@ -22117,7 +22117,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.06011845</v>
+        <v>0.05915634</v>
       </c>
     </row>
     <row r="22">
@@ -22127,7 +22127,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.23007679</v>
+        <v>0.23171845</v>
       </c>
     </row>
     <row r="23">
@@ -22137,7 +22137,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>116.64835414</v>
+        <v>115.75066594</v>
       </c>
     </row>
     <row r="24">
@@ -22147,7 +22147,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.07617235999999999</v>
+        <v>0.07573268</v>
       </c>
     </row>
     <row r="25">
@@ -22157,7 +22157,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.05969575</v>
+        <v>0.05956923</v>
       </c>
     </row>
     <row r="26">
@@ -22167,7 +22167,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.00903178</v>
+        <v>0.009106299999999999</v>
       </c>
     </row>
     <row r="27">
@@ -22177,7 +22177,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.03647589</v>
+        <v>0.03603146</v>
       </c>
     </row>
     <row r="28">
@@ -22187,27 +22187,27 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.38449204</v>
+        <v>0.39326947</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ACH</t>
+          <t>SPELL</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.03386861</v>
+        <v>0.00121699</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SPELL</t>
+          <t>ACH</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.00116182</v>
+        <v>0.03374404</v>
       </c>
     </row>
     <row r="31">
@@ -22217,37 +22217,37 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.17793724</v>
+        <v>0.18211333</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TRAC</t>
+          <t>CLV</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4.17479172</v>
+        <v>0.10456288</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CLV</t>
+          <t>GODS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.10572851</v>
+        <v>0.2945233</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GODS</t>
+          <t>TRAC</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.29279337</v>
+        <v>3.85203557</v>
       </c>
     </row>
     <row r="35">
@@ -22257,17 +22257,17 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.08835073</v>
+        <v>0.08714183</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>FARM</t>
+          <t>SUKU</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>105.26056</v>
+        <v>0.27812292</v>
       </c>
     </row>
     <row r="37">
@@ -22277,27 +22277,27 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.10661435</v>
+        <v>0.10566748</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>FIDA</t>
+          <t>FARM</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.46123181</v>
+        <v>93.10809872</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SUKU</t>
+          <t>FIDA</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.24116024</v>
+        <v>0.45343704</v>
       </c>
     </row>
     <row r="40">
@@ -22307,7 +22307,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.03041209</v>
+        <v>0.02936745</v>
       </c>
     </row>
     <row r="41">
@@ -22317,7 +22317,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.03870927</v>
+        <v>0.03724248</v>
       </c>
     </row>
     <row r="42">
@@ -22327,7 +22327,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.01216481</v>
+        <v>0.01103437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>